<commit_message>
AI+ Topic 1 Proposal
</commit_message>
<xml_diff>
--- a/pdf-scan/rules/issues_rules.xlsx
+++ b/pdf-scan/rules/issues_rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamo/mac_local/python_workspace/ai_plus/pdf-scan/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6609FC-C570-694A-8881-5D4B9F70CF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E1F3D4-7476-0746-B0FC-F168CABB9FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8640" yWindow="500" windowWidth="30040" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8360" yWindow="500" windowWidth="30040" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,12 +64,6 @@
     <t>MISS_SEC_References</t>
   </si>
   <si>
-    <t>MUST_HAVE_TIMELINE</t>
-  </si>
-  <si>
-    <t>MUST_HAVE_BUDGET</t>
-  </si>
-  <si>
     <t>Missing / odd-even-only pages</t>
   </si>
   <si>
@@ -121,9 +115,6 @@
     <t>References</t>
   </si>
   <si>
-    <t>MUST_HAVE_VALUE</t>
-  </si>
-  <si>
     <t>\b(value of the study|value of study|significance|importance|contribution|novelty|innovation)\b</t>
   </si>
   <si>
@@ -142,7 +133,16 @@
     <t>\b(objectives?|aims?|purpose|goals?|study objectives?|specific objectives?)\b</t>
   </si>
   <si>
-    <t>MUST_HAVE_OBJECTIVES</t>
+    <t>MISSING_OBJECTIVES</t>
+  </si>
+  <si>
+    <t>MISSING_BUDGET</t>
+  </si>
+  <si>
+    <t>MISSING_TIMELINE</t>
+  </si>
+  <si>
+    <t>MISSING_VALUEOFSTUDY</t>
   </si>
 </sst>
 </file>
@@ -513,7 +513,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -555,199 +555,199 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
       <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
         <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
       <c r="F7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
-      </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
-        <v>39</v>
-      </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Office Mac - For Project - Data Centre Migration
</commit_message>
<xml_diff>
--- a/pdf-scan/rules/issues_rules.xlsx
+++ b/pdf-scan/rules/issues_rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamo/mac_local/python_workspace/ai_plus/pdf-scan/rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barrytji/git/ai_plus/pdf-scan/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E1F3D4-7476-0746-B0FC-F168CABB9FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53830B01-5185-AC48-AE57-A1B574E5675B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8360" yWindow="500" windowWidth="30040" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>IssueID</t>
   </si>
@@ -46,9 +46,6 @@
     <t>SectionRegex</t>
   </si>
   <si>
-    <t>MISSING_PAGES</t>
-  </si>
-  <si>
     <t>MISS_SEC_Title</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>MISS_SEC_References</t>
   </si>
   <si>
-    <t>Missing / odd-even-only pages</t>
-  </si>
-  <si>
     <t>Missing Title section</t>
   </si>
   <si>
@@ -82,21 +76,9 @@
     <t>Missing References section</t>
   </si>
   <si>
-    <t>missing_pages</t>
-  </si>
-  <si>
     <t>missing_section</t>
   </si>
   <si>
-    <t>keyword</t>
-  </si>
-  <si>
-    <t>\b(timeline|time\s*line|schedule|gantt|milestones?|work\s*plan|workplan)\b</t>
-  </si>
-  <si>
-    <t>\b(budget|costs?|expenditure|expenses?|funding)\b</t>
-  </si>
-  <si>
     <t>any</t>
   </si>
   <si>
@@ -113,36 +95,6 @@
   </si>
   <si>
     <t>References</t>
-  </si>
-  <si>
-    <t>\b(value of the study|value of study|significance|importance|contribution|novelty|innovation)\b</t>
-  </si>
-  <si>
-    <t>Missing Value of the study</t>
-  </si>
-  <si>
-    <t>Missing Budget/cost</t>
-  </si>
-  <si>
-    <t>Missing Timeline/schedule</t>
-  </si>
-  <si>
-    <t>Missing specific study objectives</t>
-  </si>
-  <si>
-    <t>\b(objectives?|aims?|purpose|goals?|study objectives?|specific objectives?)\b</t>
-  </si>
-  <si>
-    <t>MISSING_OBJECTIVES</t>
-  </si>
-  <si>
-    <t>MISSING_BUDGET</t>
-  </si>
-  <si>
-    <t>MISSING_TIMELINE</t>
-  </si>
-  <si>
-    <t>MISSING_VALUEOFSTUDY</t>
   </si>
 </sst>
 </file>
@@ -510,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -555,199 +507,102 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
         <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>